<commit_message>
Revert "Merge pull request #48 from LakeFishing/main"
This reverts commit 660d43c6f0e5313f34b42ec314e0d333bf4f19fb, reversing
changes made to 60731923a8a563eb9061fadec661fd83d7dc8260.
</commit_message>
<xml_diff>
--- a/data_excel/193.xlsx
+++ b/data_excel/193.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Lab Test\神經網路\makedata\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ailab-master\ailab-master\ai-lab\data_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+  <si>
+    <t>數</t>
+  </si>
   <si>
     <t>v</t>
   </si>
@@ -530,132 +533,132 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C11"/>
+      <selection activeCell="G1" activeCellId="6" sqref="A5:C5 A7 B7 C7 E1 F1 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -663,17 +666,26 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge pull request #48 from LakeFishing/main""
This reverts commit 071ceee82beaf082e892f877022e6f1f84a79e42.
</commit_message>
<xml_diff>
--- a/data_excel/193.xlsx
+++ b/data_excel/193.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ailab-master\ailab-master\ai-lab\data_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Lab Test\神經網路\makedata\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
-  <si>
-    <t>數</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>v</t>
   </si>
@@ -533,132 +530,132 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" activeCellId="6" sqref="A5:C5 A7 B7 C7 E1 F1 G1"/>
+      <selection activeCell="B8" sqref="B8:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -666,26 +663,17 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>